<commit_message>
Uploaded all v2 files
This commit all v2 edits that I have been producing offline. v2 is my current working version of CCHF and will be the basis of future edits.
</commit_message>
<xml_diff>
--- a/CCHF_field_names.xlsx
+++ b/CCHF_field_names.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="18740" yWindow="5200" windowWidth="15680" windowHeight="18380" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="sLand" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="170">
   <si>
     <t>Field Name</t>
   </si>
@@ -519,6 +519,18 @@
   </si>
   <si>
     <t>velocity</t>
+  </si>
+  <si>
+    <t>cnsb</t>
+  </si>
+  <si>
+    <t>Snow sublimation</t>
+  </si>
+  <si>
+    <t>m / m^2</t>
+  </si>
+  <si>
+    <t>Depth of snow (in water equivalent) that is lost due to sublimation. Needed for full water balance.</t>
   </si>
 </sst>
 </file>
@@ -1279,10 +1291,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:E42"/>
+  <dimension ref="A4:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1319,7 +1331,7 @@
         <v>46</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>161</v>
@@ -1353,7 +1365,7 @@
         <v>48</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>162</v>
@@ -1400,7 +1412,7 @@
         <v>71</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>163</v>
@@ -1432,7 +1444,7 @@
         <v>73</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>164</v>
@@ -1443,133 +1455,138 @@
     </row>
     <row r="13" spans="1:5" ht="60">
       <c r="A13" t="s">
+        <v>166</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="60">
+      <c r="A14" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="D13" s="4" t="s">
+      <c r="C14" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="30">
-      <c r="A14" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C14" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" ht="30">
       <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" ht="30">
+      <c r="A16" t="s">
         <v>60</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="C15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="C16" t="s">
         <v>26</v>
       </c>
+      <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="30">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C17" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="18" spans="1:5" ht="30">
       <c r="A18" t="s">
-        <v>159</v>
+        <v>62</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>158</v>
+        <v>121</v>
       </c>
       <c r="C18" t="s">
         <v>26</v>
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" ht="30">
       <c r="A19" t="s">
-        <v>157</v>
-      </c>
-      <c r="B19" t="s">
-        <v>156</v>
+        <v>159</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="C19" t="s">
         <v>26</v>
       </c>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" ht="30">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>152</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>153</v>
+        <v>157</v>
+      </c>
+      <c r="B20" t="s">
+        <v>156</v>
       </c>
       <c r="C20" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>117</v>
-      </c>
+      <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" ht="30">
       <c r="A21" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C21" t="s">
         <v>26</v>
       </c>
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="E21" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="30">
       <c r="A22" t="s">
-        <v>63</v>
+        <v>154</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>122</v>
+        <v>155</v>
       </c>
       <c r="C22" t="s">
         <v>26</v>
@@ -1578,77 +1595,72 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C23" t="s">
         <v>26</v>
       </c>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5" ht="30">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C24" t="s">
         <v>26</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>125</v>
-      </c>
+      <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5" ht="30">
       <c r="A25" t="s">
-        <v>142</v>
+        <v>65</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="C25" t="s">
-        <v>106</v>
-      </c>
-      <c r="E25" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="26" spans="1:5" ht="30">
       <c r="A26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C26" t="s">
         <v>106</v>
       </c>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:5" ht="90">
+    <row r="27" spans="1:5" ht="30">
       <c r="A27" t="s">
+        <v>143</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C27" t="s">
+        <v>106</v>
+      </c>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" ht="90">
+      <c r="A28" t="s">
         <v>69</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="C27" t="s">
-        <v>160</v>
-      </c>
-      <c r="D27" t="s">
-        <v>164</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="30">
-      <c r="A28" t="s">
-        <v>66</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="C28" t="s">
         <v>160</v>
@@ -1656,14 +1668,16 @@
       <c r="D28" t="s">
         <v>164</v>
       </c>
-      <c r="E28" s="2"/>
+      <c r="E28" s="2" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="29" spans="1:5" ht="30">
       <c r="A29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C29" t="s">
         <v>160</v>
@@ -1673,55 +1687,56 @@
       </c>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:5" ht="60">
+    <row r="30" spans="1:5" ht="30">
       <c r="A30" t="s">
-        <v>68</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C30" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C30" t="s">
         <v>160</v>
       </c>
       <c r="D30" t="s">
         <v>164</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:5" ht="60">
+      <c r="A31" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D31" t="s">
+        <v>164</v>
+      </c>
+      <c r="E31" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
-      <c r="B31" s="4"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-    </row>
-    <row r="32" spans="1:5" ht="30">
-      <c r="A32" t="s">
-        <v>72</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="D32" t="s">
-        <v>164</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>131</v>
-      </c>
+    <row r="32" spans="1:5">
+      <c r="B32" s="4"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
     </row>
     <row r="33" spans="1:5" ht="30">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>72</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>18</v>
+        <v>160</v>
+      </c>
+      <c r="D33" t="s">
+        <v>164</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>131</v>
@@ -1729,13 +1744,13 @@
     </row>
     <row r="34" spans="1:5" ht="30">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>109</v>
+        <v>18</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>131</v>
@@ -1743,10 +1758,10 @@
     </row>
     <row r="35" spans="1:5" ht="30">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>109</v>
@@ -1757,16 +1772,13 @@
     </row>
     <row r="36" spans="1:5" ht="30">
       <c r="A36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D36" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>131</v>
@@ -1774,16 +1786,16 @@
     </row>
     <row r="37" spans="1:5" ht="30">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D37" t="s">
-        <v>137</v>
+        <v>105</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>131</v>
@@ -1791,46 +1803,63 @@
     </row>
     <row r="38" spans="1:5" ht="30">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C38" t="s">
-        <v>18</v>
+        <v>138</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D38" t="s">
+        <v>137</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
-      <c r="B39" s="2"/>
-      <c r="E39" s="2"/>
-    </row>
-    <row r="40" spans="1:5" ht="30">
-      <c r="A40" t="s">
-        <v>41</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>140</v>
-      </c>
+    <row r="39" spans="1:5" ht="30">
+      <c r="A39" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C39" t="s">
+        <v>18</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="B40" s="2"/>
+      <c r="E40" s="2"/>
     </row>
     <row r="41" spans="1:5" ht="30">
       <c r="A41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
-      <c r="E42" s="2"/>
+    <row r="42" spans="1:5" ht="30">
+      <c r="A42" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="E43" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>